<commit_message>
upload file & download temp, basic get requests
</commit_message>
<xml_diff>
--- a/public/files/template_analisis_makro.xlsx
+++ b/public/files/template_analisis_makro.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\14i5WMEHNCcykujaoelKsuGUih9upMyU6\JGo Files\PROJECT\Kalkulator Produktivitas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47200DBF-2E8D-4C9D-9AB2-715E9E5B181B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2AA77A-3905-44D3-A795-32CBAF0E4896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="1020" windowWidth="22524" windowHeight="11940" activeTab="2" xr2:uid="{98E8AC00-8B80-4C06-84D5-5F7DDAE11575}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{98E8AC00-8B80-4C06-84D5-5F7DDAE11575}"/>
   </bookViews>
   <sheets>
     <sheet name="data_provinsi" sheetId="2" r:id="rId1"/>
-    <sheet name="data_kota" sheetId="3" r:id="rId2"/>
-    <sheet name="(isi nama kota)" sheetId="1" r:id="rId3"/>
+    <sheet name="data_sensus_kota" sheetId="3" r:id="rId2"/>
+    <sheet name="data_kota_1" sheetId="1" r:id="rId3"/>
+    <sheet name="data_kota_2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
   <si>
     <t>Kode Lapangan Usaha</t>
   </si>
@@ -151,24 +152,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Produktivitas (Rupiah)</t>
-  </si>
-  <si>
-    <t>Growth Produktivitas Tenaga Kerja (%)</t>
-  </si>
-  <si>
-    <t>Upah (Rupiah)</t>
-  </si>
-  <si>
-    <t>Jam Kerja (Jam)</t>
-  </si>
-  <si>
-    <t>Growth Upah (%)</t>
-  </si>
-  <si>
-    <t>Growth Jam Kerja (%)</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -268,7 +251,7 @@
     <t>Jumlah Rata-Rata Jam Kerja/Pekerja</t>
   </si>
   <si>
-    <t>Upah</t>
+    <t>nama kota</t>
   </si>
 </sst>
 </file>
@@ -367,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -393,13 +376,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -410,6 +389,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -435,13 +417,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>1577340</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -459,6 +441,78 @@
         <a:xfrm>
           <a:off x="53340" y="4358640"/>
           <a:ext cx="2476500" cy="335280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" kern="1200"/>
+            <a:t>*Contoh pengisian</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1577340</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B247ED55-9CF5-4985-BCF2-7F0983D59375}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="53340" y="4754880"/>
+          <a:ext cx="2156460" cy="335280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -838,68 +892,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="15"/>
+      <c r="A1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="21"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B2" s="14"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B3" s="14"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B4" s="14"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B8" s="14"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B9" s="14"/>
     </row>
     <row r="10" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B10" s="14"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B11" s="14"/>
     </row>
@@ -926,56 +980,56 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -985,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B4BFB8-BAEC-4741-8ABE-DAFDADCAA6A3}">
-  <dimension ref="A1:AC28"/>
+  <dimension ref="A1:AC30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1012,137 +1066,59 @@
     <col min="27" max="29" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-      <c r="Y1" s="20"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="7"/>
-      <c r="W2" s="7"/>
-      <c r="X2" s="7"/>
-      <c r="Y2" s="7"/>
-      <c r="Z2" s="9"/>
-      <c r="AA2" s="9"/>
-      <c r="AB2" s="9"/>
-      <c r="AC2" s="9"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="9"/>
-      <c r="AA3" s="9"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
+      <c r="C3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1174,10 +1150,10 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1209,10 +1185,10 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1244,11 +1220,15 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -1275,10 +1255,10 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1310,15 +1290,11 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+        <v>13</v>
+      </c>
       <c r="G9" s="6"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
@@ -1345,10 +1321,10 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1380,10 +1356,10 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1415,10 +1391,10 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1450,10 +1426,10 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1485,10 +1461,10 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1520,10 +1496,10 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1555,10 +1531,10 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1590,10 +1566,10 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1625,13 +1601,13 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="10"/>
+      <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -1639,7 +1615,7 @@
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
-      <c r="L18" s="5"/>
+      <c r="L18" s="4"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
@@ -1659,9 +1635,11 @@
       <c r="AC18" s="9"/>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="11" t="s">
-        <v>36</v>
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1691,327 +1669,1121 @@
       <c r="AB19" s="9"/>
       <c r="AC19" s="9"/>
     </row>
-    <row r="25" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+    </row>
+    <row r="27" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I25" t="s">
-        <v>39</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="L25" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="2"/>
-      <c r="R25" s="2"/>
-      <c r="S25" s="2"/>
-      <c r="T25" s="2"/>
-      <c r="U25" s="2"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="2"/>
-      <c r="AA25" s="2"/>
-      <c r="AB25" s="2"/>
-      <c r="AC25" s="2"/>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="6">
-        <v>366721620.43414718</v>
-      </c>
-      <c r="D26" s="6">
-        <v>431603329.10878879</v>
-      </c>
-      <c r="E26" s="6">
-        <v>507856711.38114667</v>
-      </c>
-      <c r="F26" s="6">
-        <v>473472925</v>
-      </c>
-      <c r="G26" s="6">
-        <v>423929791.00555938</v>
-      </c>
-      <c r="H26" s="7">
-        <v>-0.30289004349437615</v>
-      </c>
-      <c r="I26" s="18">
-        <v>-0.15786285768055477</v>
-      </c>
-      <c r="J26" s="7">
-        <v>-0.14113000000000001</v>
-      </c>
-      <c r="K26" s="7">
-        <v>0.3204187302655776</v>
-      </c>
-      <c r="L26" s="4">
-        <v>4.4551399536419938</v>
-      </c>
-      <c r="M26" s="8">
-        <v>1.6730415672569743</v>
-      </c>
-      <c r="N26" s="8">
-        <v>1.7538749359909289</v>
-      </c>
-      <c r="O26" s="8">
-        <v>0.98716000000000004</v>
-      </c>
-      <c r="P26" s="8">
-        <v>1.2476023778249006</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>31939.336472004063</v>
-      </c>
-      <c r="R26" s="6">
-        <v>26570.014933304472</v>
-      </c>
-      <c r="S26" s="6">
-        <v>24356.990317326647</v>
-      </c>
-      <c r="T26" s="6">
-        <v>19829</v>
-      </c>
-      <c r="U26" s="6">
-        <v>25151.861902395663</v>
-      </c>
-      <c r="V26" s="7">
-        <v>-0.62446935790000002</v>
-      </c>
-      <c r="W26" s="7">
-        <v>4.8315218409999999E-2</v>
-      </c>
-      <c r="X26" s="7">
-        <v>-0.43715485079999999</v>
-      </c>
-      <c r="Y26" s="7">
-        <v>0.26382995440000001</v>
-      </c>
-      <c r="Z26" s="9">
-        <v>-0.1681099901</v>
-      </c>
-      <c r="AA26" s="9">
-        <v>-8.3290303809999994E-2</v>
-      </c>
-      <c r="AB26" s="9">
-        <v>-0.18590106000000001</v>
-      </c>
-      <c r="AC26" s="9">
-        <v>0.2684382421</v>
-      </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="6">
-        <v>1049374171.2902765</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1106277745.7949705</v>
-      </c>
-      <c r="E27" s="6">
-        <v>1008530471.1541885</v>
-      </c>
-      <c r="F27" s="6">
-        <v>1476059591</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1297950049.6125996</v>
-      </c>
-      <c r="H27" s="7">
-        <v>0.54528492577263776</v>
-      </c>
-      <c r="I27" s="18">
-        <v>0.30641598680484194</v>
-      </c>
-      <c r="J27" s="7">
-        <v>-0.41588999999999998</v>
-      </c>
-      <c r="K27" s="7">
-        <v>6.8371744870099546E-2</v>
-      </c>
-      <c r="L27" s="4">
-        <v>0.87370172072618013</v>
-      </c>
-      <c r="M27" s="8">
-        <v>1.6742632297608773</v>
-      </c>
-      <c r="N27" s="8">
-        <v>1.9481186171821117</v>
-      </c>
-      <c r="O27" s="8">
-        <v>1.65099</v>
-      </c>
-      <c r="P27" s="8">
-        <v>1.1298283246523775</v>
-      </c>
-      <c r="Q27" s="6">
-        <v>50435.221098507012</v>
-      </c>
-      <c r="R27" s="6">
-        <v>76474.141964828057</v>
-      </c>
-      <c r="S27" s="6">
-        <v>125073.03352080598</v>
-      </c>
-      <c r="T27" s="6">
-        <v>64025</v>
-      </c>
-      <c r="U27" s="6">
-        <v>66393.16789157514</v>
-      </c>
-      <c r="V27" s="7">
-        <v>0.9162869776</v>
-      </c>
-      <c r="W27" s="7">
-        <v>0.16356770100000001</v>
-      </c>
-      <c r="X27" s="7">
-        <v>-0.15252080370000001</v>
-      </c>
-      <c r="Y27" s="7">
-        <v>-0.31566616110000001</v>
-      </c>
-      <c r="Z27" s="9">
-        <v>0.51628445950000001</v>
-      </c>
-      <c r="AA27" s="9">
-        <v>0.63549443390000004</v>
-      </c>
-      <c r="AB27" s="9">
-        <v>-0.48809908740000002</v>
-      </c>
-      <c r="AC27" s="9">
-        <v>3.6988174800000002E-2</v>
-      </c>
+      <c r="C27" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>48</v>
+        <v>37</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C28" s="6">
+        <v>366721620.43414718</v>
+      </c>
+      <c r="D28" s="6">
+        <v>431603329.10878879</v>
+      </c>
+      <c r="E28" s="6">
+        <v>507856711.38114667</v>
+      </c>
+      <c r="F28" s="6">
+        <v>473472925</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1049374171.2902765</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1106277745.7949705</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1008530471.1541885</v>
+      </c>
+      <c r="F29" s="6">
+        <v>1476059591</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="9"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="6">
         <v>235873069.37808004</v>
       </c>
+      <c r="D30" s="6">
+        <v>249617596.27842575</v>
+      </c>
+      <c r="E30" s="6">
+        <v>227838469.4306193</v>
+      </c>
+      <c r="F30" s="6">
+        <v>236685899</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+      <c r="AB30" s="9"/>
+      <c r="AC30" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E35F16-65D6-4A11-8EA2-E6DF67C395C2}">
+  <dimension ref="A1:AC30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="7.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" s="12" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="20"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="20"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="18"/>
+      <c r="W3" s="18"/>
+      <c r="X3" s="18"/>
+      <c r="Y3" s="18"/>
+      <c r="Z3" s="20"/>
+      <c r="AA3" s="20"/>
+      <c r="AB3" s="20"/>
+      <c r="AC3" s="20"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="9"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6"/>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6"/>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6"/>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6"/>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6"/>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6"/>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+    </row>
+    <row r="27" spans="1:29" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E27" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="2"/>
+      <c r="AA27" s="2"/>
+      <c r="AB27" s="2"/>
+      <c r="AC27" s="2"/>
+    </row>
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="6">
+        <v>366721620.43414718</v>
+      </c>
       <c r="D28" s="6">
+        <v>431603329.10878879</v>
+      </c>
+      <c r="E28" s="6">
+        <v>507856711.38114667</v>
+      </c>
+      <c r="F28" s="6">
+        <v>473472925</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+    </row>
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1049374171.2902765</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1106277745.7949705</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1008530471.1541885</v>
+      </c>
+      <c r="F29" s="6">
+        <v>1476059591</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="8"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="9"/>
+    </row>
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="6">
+        <v>235873069.37808004</v>
+      </c>
+      <c r="D30" s="6">
         <v>249617596.27842575</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E30" s="6">
         <v>227838469.4306193</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F30" s="6">
         <v>236685899</v>
       </c>
-      <c r="G28" s="6">
-        <v>261332622.29347718</v>
-      </c>
-      <c r="H28" s="7">
-        <v>2.3452897513510634E-2</v>
-      </c>
-      <c r="I28" s="18">
-        <v>3.9288256941427999E-2</v>
-      </c>
-      <c r="J28" s="7">
-        <v>4.8379999999999999E-2</v>
-      </c>
-      <c r="K28" s="7">
-        <v>0.15099341327426263</v>
-      </c>
-      <c r="L28" s="4">
-        <v>8.4888490299248787</v>
-      </c>
-      <c r="M28" s="8">
-        <v>8.5864426412906081</v>
-      </c>
-      <c r="N28" s="8">
-        <v>9.151683998740662</v>
-      </c>
-      <c r="O28" s="8">
-        <v>7.9920600000000004</v>
-      </c>
-      <c r="P28" s="8">
-        <v>7.6754221160744383</v>
-      </c>
-      <c r="Q28" s="6">
-        <v>153762.52098456229</v>
-      </c>
-      <c r="R28" s="6">
-        <v>153765.50611388672</v>
-      </c>
-      <c r="S28" s="6">
-        <v>175060.93624586595</v>
-      </c>
-      <c r="T28" s="6">
-        <v>177178</v>
-      </c>
-      <c r="U28" s="6">
-        <v>196216.39325220129</v>
-      </c>
-      <c r="V28" s="7">
-        <v>1.1496683590000001E-2</v>
-      </c>
-      <c r="W28" s="7">
-        <v>6.5829515330000005E-2</v>
-      </c>
-      <c r="X28" s="7">
-        <v>-0.12671154279999999</v>
-      </c>
-      <c r="Y28" s="7">
-        <v>-3.9619057409999998E-2</v>
-      </c>
-      <c r="Z28" s="9">
-        <v>1.9413894269999999E-5</v>
-      </c>
-      <c r="AA28" s="9">
-        <v>0.1384928953</v>
-      </c>
-      <c r="AB28" s="9">
-        <v>1.209329619E-2</v>
-      </c>
-      <c r="AC28" s="9">
-        <v>0.10745348320000001</v>
-      </c>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="8"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+      <c r="AB30" s="9"/>
+      <c r="AC30" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>